<commit_message>
add custom lib and flake8
</commit_message>
<xml_diff>
--- a/output/~dicom_tag_dumps.xlsx
+++ b/output/~dicom_tag_dumps.xlsx
@@ -171,7 +171,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -595,6 +616,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I65536"/>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="OT">
+      <formula>NOT(ISERROR(SEARCH("OT",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F4">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Physicists">
+      <formula>NOT(ISERROR(SEARCH("Physicists",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add dicom_tools, package updates
</commit_message>
<xml_diff>
--- a/output/~dicom_tag_dumps.xlsx
+++ b/output/~dicom_tag_dumps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>filename:</t>
   </si>
@@ -70,6 +70,9 @@
     <t>TSHOW</t>
   </si>
   <si>
+    <t>LittleEndianImplicit</t>
+  </si>
+  <si>
     <t>dcmtk_dump_src.txt</t>
   </si>
   <si>
@@ -92,6 +95,9 @@
   </si>
   <si>
     <t>SOMATOM Definition Edge</t>
+  </si>
+  <si>
+    <t>JPEGLossless:Non-hierarchical-1stOrderPrediction</t>
   </si>
   <si>
     <t>fuji_dicom_dump.txt</t>
@@ -499,7 +505,7 @@
     <col min="6" max="6" width="58.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -556,62 +562,66 @@
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>